<commit_message>
Add missing files to Jun27_25 update
</commit_message>
<xml_diff>
--- a/Protocols/-80_Freezer.xlsx
+++ b/Protocols/-80_Freezer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geoffreyhorsman/Dropbox/WLU/Research/Frozen stocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geoffreyhorsman/Dropbox/WLU/Gitweb/horsmanlab.github.io/Protocols/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AEFB5A-CC03-254F-9B71-7C1B51434A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339B8EDD-289A-FF4E-9A73-587C5ECCB300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21100" windowWidth="38400" windowHeight="20540" activeTab="1" xr2:uid="{3ABAE8F3-DCF4-7844-BCB9-000C496DFAAC}"/>
+    <workbookView xWindow="-4720" yWindow="-21100" windowWidth="35300" windowHeight="19640" activeTab="1" xr2:uid="{3ABAE8F3-DCF4-7844-BCB9-000C496DFAAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="972">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1558" uniqueCount="973">
   <si>
     <t xml:space="preserve">Box 1 </t>
   </si>
@@ -3372,12 +3372,15 @@
   <si>
     <t>DH5a pET28 RiPP-PP (RiPP precursor peptide)</t>
   </si>
+  <si>
+    <t>"ppm-c"—DH5a stock of pET28 containing Ppm from Mytilus edulis (UniProt P56839); synthesized June 2025 as NdeI/XhoI fragment in pET28</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3396,6 +3399,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3424,10 +3435,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3460,8 +3472,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3486,9 +3500,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3526,7 +3540,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3632,7 +3646,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3774,7 +3788,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -10775,12 +10789,11 @@
       <c r="DO36" s="2">
         <v>2</v>
       </c>
-      <c r="DV36" s="8" t="s">
-        <v>227</v>
+      <c r="DU36" s="14" t="s">
+        <v>972</v>
       </c>
       <c r="DW36" s="2">
-        <f>SUM(DW3:DW35)</f>
-        <v>55</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="5:127" x14ac:dyDescent="0.2">
@@ -10866,6 +10879,13 @@
       </c>
       <c r="DO37" s="2">
         <v>2</v>
+      </c>
+      <c r="DV37" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="DW37" s="2">
+        <f>SUM(DW3:DW36)</f>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="5:127" x14ac:dyDescent="0.2">
@@ -11552,6 +11572,9 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="EK3:EM13">
     <sortCondition ref="EK3:EK13"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="DU36" r:id="rId1" xr:uid="{7172E0A9-7D74-FC49-9EC9-769956BC5C73}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="B3:B4 B5:B10 B11:B27 F3:F45 N3:N37 R8:R30 Z4 AD3:AD30 AH3:AH53 AL3:AL44 AP3:AP16 AT3:AT41 AX3:AX13 BB6 BF6:BF23 BN5:BN35 BR3:BR35 BV3:BV52 BZ3:BZ15 CD3:CD4 CH3:CH27 CL3:CL25 CP3:CP45 CT3:CT24 DB4:DB25 DV19:DV32 DZ3 ED5:ED15 EH6:EH11" numberStoredAsText="1"/>

</xml_diff>